<commit_message>
Atualização automática de SALTO_DO_JACUI.xlsx
</commit_message>
<xml_diff>
--- a/SALTO_DO_JACUI.xlsx
+++ b/SALTO_DO_JACUI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D2C1B71-A3BE-4723-B4E0-4BDB44799EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08EC729C-D63E-426C-9F6F-E1E358E7BA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1269,7 +1269,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{ED327A64-10D8-4AB1-A543-5FE40068D874}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{97EB71F8-CA24-41CF-BB17-1D6AFE0F8E15}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1299,10 +1299,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E954DF-72E2-4F8A-9FD3-29458FA8B9D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9097B44C-3B1D-4700-98F3-CCE386F3970C}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1340,7 +1340,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B84E3F-E95A-4C12-88AF-2A4C487B6089}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30C7E35C-29F6-49F7-AB10-5C01969C9557}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1403,7 +1403,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEF08816-A77A-4005-A5FB-1548166717F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E6DCB02-223E-4A77-A082-9E31D744EA05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1422,7 +1422,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F5125D-D2F0-ED25-6CD1-6535719DE51F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDA5E22D-8044-C088-F53E-FFFED2135C9A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C03BEEA-78E1-7BF7-57FC-07D1FBA9F40B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA4DDD09-FF58-B1A6-0070-2F1BF20739F4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{133B3573-4981-AB07-C664-823E584B77DE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDB58192-6F33-BFDC-86FB-41B3243EB278}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1521,7 +1521,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2148C64B-FCFE-2110-A3A1-5B4928883F25}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB5C9CB1-B957-585A-9D8A-B31F758DD80D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1552,7 +1552,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C3F3528-5D6E-FC3E-E8EA-32BC64664052}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{616D1717-57F7-106A-0746-8C5CB14ADFE8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1595,7 +1595,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AACFB4B6-D2C7-448E-BEC0-6A787535F7B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22F7BAAB-A82D-4D93-91C2-AB53C92EB12B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1633,7 +1633,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480C3145-F8F7-477D-8E86-0C7F5E56AEF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF50EFAE-1036-45A4-85C4-05831BE9F710}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1676,7 +1676,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFE33B07-7DE1-42FC-9100-A14FDE9B0A6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16F04446-F856-4A8B-821A-98D26A5AFEAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1989,7 +1989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195D1A72-9A83-40B0-B424-92AC8782D08F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C165BF43-2C3A-4805-B323-04BEBB82FD5B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>